<commit_message>
add: upload finish code
</commit_message>
<xml_diff>
--- a/Contacts/Contacts.xlsx
+++ b/Contacts/Contacts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>First Name</t>
   </si>
@@ -41,33 +41,18 @@
     <t>Stenio</t>
   </si>
   <si>
-    <t>D. Rapchan</t>
-  </si>
-  <si>
     <t>Junior</t>
   </si>
   <si>
-    <t>Fletcher</t>
-  </si>
-  <si>
-    <t>Joestar</t>
-  </si>
-  <si>
     <t>stenio.rapchan@gmail.com</t>
   </si>
   <si>
-    <t>steniodr@hotmail.com</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
     <t>Rodrigo</t>
   </si>
   <si>
-    <t>Mendes</t>
-  </si>
-  <si>
     <t>Director</t>
   </si>
   <si>
@@ -89,10 +74,55 @@
     <t>Intermediate</t>
   </si>
   <si>
-    <t>Carla</t>
-  </si>
-  <si>
-    <t>Munhoz</t>
+    <t>carlos@carlos.com.br</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Pascal</t>
+  </si>
+  <si>
+    <t>Rapchan</t>
+  </si>
+  <si>
+    <t>odelinda3848@uorak.com</t>
+  </si>
+  <si>
+    <t>Odelinda</t>
+  </si>
+  <si>
+    <t>JoJo</t>
+  </si>
+  <si>
+    <t>miltinho@gmail.com</t>
+  </si>
+  <si>
+    <t>ravi@hotmail.com</t>
+  </si>
+  <si>
+    <t>Rodrigues</t>
+  </si>
+  <si>
+    <t>roro@uol.com.br</t>
+  </si>
+  <si>
+    <t>Reginaldo</t>
+  </si>
+  <si>
+    <t>Maromba</t>
+  </si>
+  <si>
+    <t>regis100@hotmail.com</t>
+  </si>
+  <si>
+    <t>Guilhermino</t>
+  </si>
+  <si>
+    <t>Novais</t>
+  </si>
+  <si>
+    <t>guinova@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -419,16 +449,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -449,86 +479,114 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>